<commit_message>
Add numpy arrays to the simple counters
</commit_message>
<xml_diff>
--- a/streaming/simple_counters.xlsx
+++ b/streaming/simple_counters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\xlslim-code-samples\streaming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFE9F7C-9F36-4656-92C1-F909F5149485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9885EA57-80E8-4FB9-BA29-5290F5E9FFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6069" yWindow="3266" windowWidth="24685" windowHeight="13054" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
+    <workbookView xWindow="5494" yWindow="1954" windowWidth="24686" windowHeight="13055" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Workbook location</t>
   </si>
@@ -80,9 +80,19 @@
     <t>Async</t>
   </si>
   <si>
+    <t>Regular Numpy Array Counter</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Async Numpy Array Counter</t>
+  </si>
+  <si>
     <t>This workbook shows how simple generator functions can stream data into Excel using xlSlim.
 The Python module simple_counters.py has two counter functions. One is a regular Python function with a yield, which turns the function into a generator function. The second is slightly more advanced Python function that asynchronously generates values.
-Cells C6 and D6 show how the functions are exposed in Excel as regular worksheet functions, all the complexity of streaming data is taken care of internally within xlSlim.</t>
+Cells C6 and D6 show how the functions are exposed in Excel as regular worksheet functions, all the complexity of streaming data is taken care of internally within xlSlim.
+Cells A10 and C10 show how numpy arrays can be streamed into Excel. Indeed any supported objects can be streamed. Cells B13 and D13 show how the object cache handles can be passed into xlSlim functions just the same as other xlSlim functions returning cached objects.</t>
   </si>
 </sst>
 </file>
@@ -261,6 +271,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -279,7 +290,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent5" xfId="2" builtinId="47"/>
@@ -304,22 +314,40 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv_a6f06a8b5adf4d248cd54959ead9b39b">
+    <main first="rtdsrv_4ad5b0806a0d4c0c8dd356af92c2f2aa">
       <tp>
-        <v>99</v>
+        <v>49</v>
+        <stp/>
+        <stp>counter</stp>
+        <stp>50</stp>
+        <stp>2</stp>
+        <tr r="C6" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_4ad5b0806a0d4c0c8dd356af92c2f2aa">
+      <tp t="s">
+        <v>async_array_counter/50/2@50</v>
+        <stp/>
+        <stp>async_array_counter</stp>
+        <stp>50</stp>
+        <stp>2</stp>
+        <tr r="C10" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>array_counter/50/2@50</v>
+        <stp/>
+        <stp>array_counter</stp>
+        <stp>50</stp>
+        <stp>2</stp>
+        <tr r="A10" s="1"/>
+      </tp>
+      <tp>
+        <v>49</v>
         <stp/>
         <stp>async_counter</stp>
-        <stp>100</stp>
+        <stp>50</stp>
         <stp>2</stp>
         <tr r="D6" s="1"/>
-      </tp>
-      <tp>
-        <v>99</v>
-        <stp/>
-        <stp>counter</stp>
-        <stp>100</stp>
-        <stp>2</stp>
-        <tr r="C6" s="1"/>
       </tp>
     </main>
   </volType>
@@ -626,7 +654,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -645,16 +673,16 @@
         <f t="array" ref="B1">_xll.WorkbookLocation()</f>
         <v>D:\github\xlslim-code-samples\streaming</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="7"/>
+      <c r="E1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
@@ -664,14 +692,14 @@
         <f>B1&amp;"\simple_counters.py"</f>
         <v>D:\github\xlslim-code-samples\streaming\simple_counters.py</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="10"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
@@ -681,24 +709,24 @@
         <f t="array" ref="B3">_xll.RegisterPyModule(B2)</f>
         <v>Registered D:\github\xlslim-code-samples\streaming\simple_counters.py</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="10"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:12" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C5" s="5" t="s">
@@ -707,124 +735,180 @@
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="10"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="12">
-        <v>100</v>
+      <c r="B6" s="6">
+        <v>50</v>
       </c>
       <c r="C6" s="2" cm="1">
         <f t="array" ref="C6">_xll.counter(B6,B7)</f>
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2" cm="1">
         <f t="array" ref="D6">_xll.async_counter(B6,B7)</f>
-        <v>99</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="9"/>
+        <v>49</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="10"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="10"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="10"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="9"/>
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="10"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="9"/>
+      <c r="A10" s="2" t="str" cm="1">
+        <f t="array" ref="A10">_xll.array_counter(B6,B7)</f>
+        <v>array_counter/50/2@50</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="str" cm="1">
+        <f t="array" ref="C10">_xll.async_array_counter(B6,B7)</f>
+        <v>async_array_counter/50/2@50</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="10"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="9"/>
+      <c r="A11" s="2" cm="1">
+        <f t="array" ref="A11:B12">_xll.ViewPyObject(A10)</f>
+        <v>49</v>
+      </c>
+      <c r="B11" s="2">
+        <v>49</v>
+      </c>
+      <c r="C11" s="2" cm="1">
+        <f t="array" ref="C11:D12">_xll.ViewPyObject(C10)</f>
+        <v>49</v>
+      </c>
+      <c r="D11" s="2">
+        <v>49</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="10"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="9"/>
+      <c r="A12" s="2">
+        <v>49</v>
+      </c>
+      <c r="B12" s="2">
+        <v>49</v>
+      </c>
+      <c r="C12" s="2">
+        <v>49</v>
+      </c>
+      <c r="D12" s="2">
+        <v>49</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="10"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="9"/>
+      <c r="A13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2" cm="1">
+        <f t="array" ref="B13">_xll.array_sum_from_handle(A10)</f>
+        <v>196</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2" cm="1">
+        <f t="array" ref="D13">_xll.array_sum_from_handle(C10)</f>
+        <v>196</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="10"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -836,18 +920,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -983,14 +1067,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE1A4A2-BF99-4D94-B73F-D9211460B53D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B898F4E-8707-4CA2-9F8B-513D2A3B8BD6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -1002,6 +1078,14 @@
     <ds:schemaRef ds:uri="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE1A4A2-BF99-4D94-B73F-D9211460B53D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update Bloomberg and simple counters examples
</commit_message>
<xml_diff>
--- a/streaming/simple_counters.xlsx
+++ b/streaming/simple_counters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\xlslim-code-samples\streaming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B49D443-C24A-4636-BAEA-3973F1421012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953DBC2C-4F8B-4DEC-A6F1-9296B2D5CAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
+    <workbookView xWindow="6506" yWindow="2486" windowWidth="24685" windowHeight="13054" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -238,46 +238,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -286,7 +246,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -299,19 +259,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -338,39 +286,39 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv_00ce64b15fcf4cbb99fe6e824cf7bdca">
+    <main first="rtdsrv_2a05dc1e2b5242db93d1dd18b7453eb4">
       <tp>
-        <v>33</v>
+        <v>999</v>
         <stp/>
         <stp>counter</stp>
-        <stp>32003</stp>
+        <stp>32993</stp>
         <tr r="C6" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv_00ce64b15fcf4cbb99fe6e824cf7bdca">
+    <main first="rtdsrv_2a05dc1e2b5242db93d1dd18b7453eb4">
       <tp t="s">
-        <v>RTD/32003@2067</v>
+        <v>RTD/32993@3610</v>
         <stp/>
         <stp>async_array_counter</stp>
-        <stp>32003</stp>
+        <stp>32993</stp>
         <tr r="C10" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv_00ce64b15fcf4cbb99fe6e824cf7bdca">
+    <main first="rtdsrv_2a05dc1e2b5242db93d1dd18b7453eb4">
       <tp>
-        <v>33</v>
+        <v>999</v>
         <stp/>
         <stp>async_counter</stp>
-        <stp>32003</stp>
+        <stp>32993</stp>
         <tr r="D6" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv_00ce64b15fcf4cbb99fe6e824cf7bdca">
+    <main first="rtdsrv_2a05dc1e2b5242db93d1dd18b7453eb4">
       <tp t="s">
-        <v>RTD/32003@2068</v>
+        <v>RTD/32993@4000</v>
         <stp/>
         <stp>array_counter</stp>
-        <stp>32003</stp>
+        <stp>32993</stp>
         <tr r="A10" s="1"/>
       </tp>
     </main>
@@ -675,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774E7E1C-D275-4DD4-9028-FA14541EA3B8}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -706,7 +654,7 @@
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
-      <c r="L1" s="8"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
@@ -716,14 +664,14 @@
         <f>B1&amp;"\simple_counters.py"</f>
         <v>D:\github\xlslim-code-samples\streaming\simple_counters.py</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="10"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
@@ -733,24 +681,24 @@
         <f t="array" ref="B3">_xll.RegisterPyModule(B2)</f>
         <v>Registered D:\github\xlslim-code-samples\streaming\simple_counters.py</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="10"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="10"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
     </row>
     <row r="5" spans="1:12" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C5" s="5" t="s">
@@ -759,14 +707,14 @@
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="10"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
@@ -777,46 +725,46 @@
       </c>
       <c r="C6" s="2" cm="1">
         <f t="array" ref="C6">_xll.counter(B6,B7)</f>
-        <v>33</v>
+        <v>999</v>
       </c>
       <c r="D6" s="2" cm="1">
         <f t="array" ref="D6">_xll.async_counter(B6,B7)</f>
-        <v>33</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="10"/>
+        <v>999</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="6">
-        <v>10</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="10"/>
+        <v>1000</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="10"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
@@ -825,80 +773,80 @@
       <c r="C9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="10"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="str" cm="1">
         <f t="array" ref="A10">_xll.array_counter(B6,B7)</f>
-        <v>RTD/32003@2068</v>
+        <v>RTD/32993@4000</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="str" cm="1">
         <f t="array" ref="C10">_xll.async_array_counter(B6,B7)</f>
-        <v>RTD/32003@2067</v>
+        <v>RTD/32993@3610</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="10"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="2" cm="1">
         <f t="array" ref="A11:B12">_xll.ViewPyObject(A10)</f>
-        <v>33</v>
+        <v>999</v>
       </c>
       <c r="B11" s="2">
-        <v>33</v>
+        <v>999</v>
       </c>
       <c r="C11" s="2" cm="1">
         <f t="array" ref="C11:D12">_xll.ViewPyObject(C10)</f>
-        <v>33</v>
+        <v>999</v>
       </c>
       <c r="D11" s="2">
-        <v>33</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="10"/>
+        <v>999</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="2">
-        <v>33</v>
+        <v>999</v>
       </c>
       <c r="B12" s="2">
-        <v>33</v>
+        <v>999</v>
       </c>
       <c r="C12" s="2">
-        <v>33</v>
+        <v>999</v>
       </c>
       <c r="D12" s="2">
-        <v>33</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="10"/>
+        <v>999</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
@@ -906,37 +854,57 @@
       </c>
       <c r="B13" s="2" cm="1">
         <f t="array" ref="B13">_xll.array_sum_from_handle(A10)</f>
-        <v>132</v>
+        <v>3996</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="2" cm="1">
         <f t="array" ref="D13">_xll.array_sum_from_handle(C10)</f>
-        <v>132</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="10"/>
+        <v>3996</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="12"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E1:L14"/>
+    <mergeCell ref="E1:L16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1076,18 +1044,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1109,14 +1077,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE1A4A2-BF99-4D94-B73F-D9211460B53D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B898F4E-8707-4CA2-9F8B-513D2A3B8BD6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -1130,4 +1090,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE1A4A2-BF99-4D94-B73F-D9211460B53D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Simple counters example looking good
</commit_message>
<xml_diff>
--- a/streaming/simple_counters.xlsx
+++ b/streaming/simple_counters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\xlslim-code-samples\streaming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953DBC2C-4F8B-4DEC-A6F1-9296B2D5CAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8685C00B-8ECE-4EBD-95DB-0F715579EF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6506" yWindow="2486" windowWidth="24685" windowHeight="13054" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
+    <workbookView xWindow="1114" yWindow="909" windowWidth="24686" windowHeight="13054" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -286,39 +286,37 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv_2a05dc1e2b5242db93d1dd18b7453eb4">
+    <main first="rtdsrv_fd10f3797bca4254b5a22addfd062a1e">
+      <tp t="s">
+        <v>RTD/32093@3587</v>
+        <stp/>
+        <stp>async_array_counter</stp>
+        <stp>32093</stp>
+        <tr r="C10" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_fd10f3797bca4254b5a22addfd062a1e">
+      <tp>
+        <v>999</v>
+        <stp/>
+        <stp>async_counter</stp>
+        <stp>32093</stp>
+        <tr r="D6" s="1"/>
+      </tp>
       <tp>
         <v>999</v>
         <stp/>
         <stp>counter</stp>
-        <stp>32993</stp>
+        <stp>32093</stp>
         <tr r="C6" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv_2a05dc1e2b5242db93d1dd18b7453eb4">
+    <main first="rtdsrv_fd10f3797bca4254b5a22addfd062a1e">
       <tp t="s">
-        <v>RTD/32993@3610</v>
-        <stp/>
-        <stp>async_array_counter</stp>
-        <stp>32993</stp>
-        <tr r="C10" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_2a05dc1e2b5242db93d1dd18b7453eb4">
-      <tp>
-        <v>999</v>
-        <stp/>
-        <stp>async_counter</stp>
-        <stp>32993</stp>
-        <tr r="D6" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_2a05dc1e2b5242db93d1dd18b7453eb4">
-      <tp t="s">
-        <v>RTD/32993@4000</v>
+        <v>RTD/32093@4000</v>
         <stp/>
         <stp>array_counter</stp>
-        <stp>32993</stp>
+        <stp>32093</stp>
         <tr r="A10" s="1"/>
       </tp>
     </main>
@@ -626,18 +624,18 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="21.07421875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.69140625" customWidth="1"/>
     <col min="2" max="2" width="15.84375" customWidth="1"/>
     <col min="3" max="3" width="18.69140625" customWidth="1"/>
     <col min="4" max="4" width="27.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="27.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -745,7 +743,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="6">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -785,12 +783,12 @@
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="str" cm="1">
         <f t="array" ref="A10">_xll.array_counter(B6,B7)</f>
-        <v>RTD/32993@4000</v>
+        <v>RTD/32093@4000</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="str" cm="1">
         <f t="array" ref="C10">_xll.async_array_counter(B6,B7)</f>
-        <v>RTD/32993@3610</v>
+        <v>RTD/32093@3587</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="8"/>
@@ -912,6 +910,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010056A28DAB99C48B469009752D21F8474A" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3725108ba1e248dd961cbde49d36f75">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="58a034177a2e5a667d336d2ca3036430" ns3:_="">
     <xsd:import namespace="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
@@ -1043,12 +1047,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1059,6 +1057,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B898F4E-8707-4CA2-9F8B-513D2A3B8BD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C9D94B-68A3-4C5A-8543-29DBB1AA8066}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1076,22 +1090,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B898F4E-8707-4CA2-9F8B-513D2A3B8BD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE1A4A2-BF99-4D94-B73F-D9211460B53D}">
   <ds:schemaRefs>

</xml_diff>